<commit_message>
V1.1 punctiation, bigger text
</commit_message>
<xml_diff>
--- a/CardContent.xlsx
+++ b/CardContent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uwiegaertner/GitHub/HonestMeetingCards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B532315-09CE-4B47-90F5-D0528E491BAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EE9EFE-EB32-6E40-909A-1874DE20ADE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32780" yWindow="2180" windowWidth="10000" windowHeight="17440" xr2:uid="{2AC391B4-215E-4947-8F7A-4CF7226239EB}"/>
+    <workbookView xWindow="-32780" yWindow="2180" windowWidth="29300" windowHeight="17440" xr2:uid="{2AC391B4-215E-4947-8F7A-4CF7226239EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,64 +42,64 @@
     <t>TextFrontside</t>
   </si>
   <si>
-    <t>&lt;-- That's me not caring</t>
-  </si>
-  <si>
-    <t>I pretend you are muted</t>
-  </si>
-  <si>
-    <t>I know you are doing Emails in parallel</t>
-  </si>
-  <si>
-    <t>I couldn't care less</t>
-  </si>
-  <si>
-    <t>Your hair looks funny</t>
-  </si>
-  <si>
     <t>What's the purpose of this meeting again?</t>
   </si>
   <si>
-    <t>My silence isn't approval. I was just not listening</t>
-  </si>
-  <si>
-    <t>My video is not frozen. I just try not to move</t>
-  </si>
-  <si>
-    <t>I'm just trying to stick my mouse pointer in your ear</t>
-  </si>
-  <si>
-    <t>It's too late for introducing an agenda</t>
-  </si>
-  <si>
-    <t>That will escalate quickly</t>
-  </si>
-  <si>
-    <t>Some people just want to see the world burn</t>
-  </si>
-  <si>
     <t>You already lost me at "who sent the invitation for this?"</t>
   </si>
   <si>
-    <t>You switched off your camera so I moved a funny photo over your video thumbnail</t>
-  </si>
-  <si>
     <t>Look there! A squirrel!</t>
   </si>
   <si>
     <t>Here we are now, entertain us!</t>
   </si>
   <si>
-    <t>All I hear is "mi mi mi"</t>
-  </si>
-  <si>
-    <t>Told you so</t>
-  </si>
-  <si>
-    <t>That will never scale</t>
-  </si>
-  <si>
     <t>Who hired you?</t>
+  </si>
+  <si>
+    <t>I pretend you are muted.</t>
+  </si>
+  <si>
+    <t>I know you are doing Emails in parallel.</t>
+  </si>
+  <si>
+    <t>I couldn't care less.</t>
+  </si>
+  <si>
+    <t>Your hair looks funny.</t>
+  </si>
+  <si>
+    <t>My silence isn't approval. I was just not listening.</t>
+  </si>
+  <si>
+    <t>My video is not frozen. I just try not to move.</t>
+  </si>
+  <si>
+    <t>I'm just trying to stick my cursor in your ear.</t>
+  </si>
+  <si>
+    <t>That will escalate quickly.</t>
+  </si>
+  <si>
+    <t>We ignore your agenda.</t>
+  </si>
+  <si>
+    <t>I want to see the world burn.</t>
+  </si>
+  <si>
+    <t>You switched off your camera so I moved a funny photo over your video thumbnail.</t>
+  </si>
+  <si>
+    <t>All I hear is "mi mi mi".</t>
+  </si>
+  <si>
+    <t>Told you so.</t>
+  </si>
+  <si>
+    <t>That will never scale.</t>
+  </si>
+  <si>
+    <t>← That's me not caring.</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -484,7 +484,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -492,7 +492,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -500,7 +500,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -508,7 +508,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -516,7 +516,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -532,7 +532,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -540,7 +540,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -556,7 +556,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -564,7 +564,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -572,7 +572,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -580,7 +580,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -588,7 +588,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -596,7 +596,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -628,7 +628,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
card number smaller, text card 1 'could not'
</commit_message>
<xml_diff>
--- a/CardContent.xlsx
+++ b/CardContent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uwiegaertner/GitHub/HonestMeetingCards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EE9EFE-EB32-6E40-909A-1874DE20ADE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80470865-B3EE-9E4A-8717-76E149771792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32780" yWindow="2180" windowWidth="29300" windowHeight="17440" xr2:uid="{2AC391B4-215E-4947-8F7A-4CF7226239EB}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>I know you are doing Emails in parallel.</t>
   </si>
   <si>
-    <t>I couldn't care less.</t>
-  </si>
-  <si>
     <t>Your hair looks funny.</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>← That's me not caring.</t>
+  </si>
+  <si>
+    <t>I could not care less.</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -500,7 +500,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -508,7 +508,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -532,7 +532,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -540,7 +540,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -556,7 +556,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -564,7 +564,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -580,7 +580,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -604,7 +604,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -612,7 +612,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -620,7 +620,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
version 1.2 line break and text variations
</commit_message>
<xml_diff>
--- a/CardContent.xlsx
+++ b/CardContent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uwiegaertner/GitHub/HonestMeetingCards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80470865-B3EE-9E4A-8717-76E149771792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0765B6-7E89-464F-ABCF-5E0585C17CAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32780" yWindow="2180" windowWidth="29300" windowHeight="17440" xr2:uid="{2AC391B4-215E-4947-8F7A-4CF7226239EB}"/>
   </bookViews>
@@ -45,15 +45,6 @@
     <t>What's the purpose of this meeting again?</t>
   </si>
   <si>
-    <t>You already lost me at "who sent the invitation for this?"</t>
-  </si>
-  <si>
-    <t>Look there! A squirrel!</t>
-  </si>
-  <si>
-    <t>Here we are now, entertain us!</t>
-  </si>
-  <si>
     <t>Who hired you?</t>
   </si>
   <si>
@@ -66,30 +57,12 @@
     <t>Your hair looks funny.</t>
   </si>
   <si>
-    <t>My silence isn't approval. I was just not listening.</t>
-  </si>
-  <si>
-    <t>My video is not frozen. I just try not to move.</t>
-  </si>
-  <si>
-    <t>I'm just trying to stick my cursor in your ear.</t>
-  </si>
-  <si>
     <t>That will escalate quickly.</t>
   </si>
   <si>
-    <t>We ignore your agenda.</t>
-  </si>
-  <si>
     <t>I want to see the world burn.</t>
   </si>
   <si>
-    <t>You switched off your camera so I moved a funny photo over your video thumbnail.</t>
-  </si>
-  <si>
-    <t>All I hear is "mi mi mi".</t>
-  </si>
-  <si>
     <t>Told you so.</t>
   </si>
   <si>
@@ -100,6 +73,39 @@
   </si>
   <si>
     <t>I could not care less.</t>
+  </si>
+  <si>
+    <t>I'm just trying to stick my mouse pointer in your ear.</t>
+  </si>
+  <si>
+    <t>I placed a funny photo over your switched-off video.</t>
+  </si>
+  <si>
+    <t>My silence isn't approval.
+I was just not listening.</t>
+  </si>
+  <si>
+    <t>My video is not frozen.
+I just try not to move.</t>
+  </si>
+  <si>
+    <t>You already lost me at
+"who sent the invitation for this?"</t>
+  </si>
+  <si>
+    <t>Look there!
+A squirrel!</t>
+  </si>
+  <si>
+    <t>Here we are now,
+entertain us!</t>
+  </si>
+  <si>
+    <t>All I hear is
+"mi mi mi".</t>
+  </si>
+  <si>
+    <t>Your agenda is useless.</t>
   </si>
 </sst>
 </file>
@@ -135,8 +141,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +463,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +485,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -484,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -492,7 +501,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -500,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -508,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -519,20 +528,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -540,7 +549,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -548,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -556,7 +565,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -564,15 +573,15 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -580,31 +589,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>17</v>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -612,7 +621,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -620,7 +629,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -628,7 +637,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>